<commit_message>
Commented all .class files with proper documentation
</commit_message>
<xml_diff>
--- a/F9Resource/src/Keywords/Automation Test Cases/Backup/BuyerPriceBook.xlsx
+++ b/F9Resource/src/Keywords/Automation Test Cases/Backup/BuyerPriceBook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView activeTab="6" firstSheet="2" windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
+    <workbookView activeTab="1" windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
   </bookViews>
   <sheets>
     <sheet name="TestScenarios" r:id="rId1" sheetId="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="156">
   <si>
     <t>TestScenario Id</t>
   </si>
@@ -391,100 +391,103 @@
     <t>customer</t>
   </si>
   <si>
+    <t>Qty Range is displayed</t>
+  </si>
+  <si>
+    <t>Department is not getting displayed</t>
+  </si>
+  <si>
+    <t>date Range is not getting displayed</t>
+  </si>
+  <si>
+    <t>Qty Range is not getting displayed</t>
+  </si>
+  <si>
+    <t>Unit is not getting displayed</t>
+  </si>
+  <si>
+    <t>COPYPASTEPRICEBOOK</t>
+  </si>
+  <si>
+    <t>COPYPASTEPRICEBOOKSAVE</t>
+  </si>
+  <si>
+    <t>created successfully</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verifying the customization of Price Book by adding the desired fields </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customizing the Price Book by adding the desired fields by saving the customization </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verifying the customization of Price Book by adding the existing columns </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customizing the Price Book by removing the existing columns by saving the customization </t>
+  </si>
+  <si>
+    <t>Copy &amp; Paste feature of Price Book</t>
+  </si>
+  <si>
+    <t>Buyer Price Book Home Page Close</t>
+  </si>
+  <si>
+    <t>TC016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verifying the customization of Price Book by removing the existing columns </t>
+  </si>
+  <si>
+    <t>Verify if it is able to Customize the Price book by removing the existing  column.</t>
+  </si>
+  <si>
+    <t>Verify if it is able to save the Price book by removing the provided column.</t>
+  </si>
+  <si>
+    <t>Verifying the Copy &amp; Paste feature of Price Book</t>
+  </si>
+  <si>
+    <t>Verify if it is able to Copy &amp; Paste the data from one Price Book to the New Price book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copy the existing Price book's data to a new Price book and save </t>
+  </si>
+  <si>
+    <t>Verify if it is able to save the Price book by copying  the existing Price Book's data to the new Price Book</t>
+  </si>
+  <si>
+    <t>Blocked</t>
+  </si>
+  <si>
+    <t>Price Book is empty</t>
+  </si>
+  <si>
+    <t>AUTO040119</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Price Book created successfully</t>
+  </si>
+  <si>
+    <t>Pricebook details deleted successfully.</t>
+  </si>
+  <si>
     <t>Department is displayed</t>
   </si>
   <si>
     <t>date Range is displayed</t>
   </si>
   <si>
-    <t>Qty Range is displayed</t>
+    <t>There are no updates in price book</t>
   </si>
   <si>
     <t>Unit is displayed</t>
-  </si>
-  <si>
-    <t>Department is not getting displayed</t>
-  </si>
-  <si>
-    <t>date Range is not getting displayed</t>
-  </si>
-  <si>
-    <t>Qty Range is not getting displayed</t>
-  </si>
-  <si>
-    <t>Unit is not getting displayed</t>
-  </si>
-  <si>
-    <t>COPYPASTEPRICEBOOK</t>
-  </si>
-  <si>
-    <t>COPYPASTEPRICEBOOKSAVE</t>
-  </si>
-  <si>
-    <t>created successfully</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Blocked</t>
-  </si>
-  <si>
-    <t>Price Book created successfully</t>
-  </si>
-  <si>
-    <t>AUTO110918</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verifying the customization of Price Book by adding the desired fields </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customizing the Price Book by adding the desired fields by saving the customization </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verifying the customization of Price Book by adding the existing columns </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customizing the Price Book by removing the existing columns by saving the customization </t>
-  </si>
-  <si>
-    <t>Copy &amp; Paste feature of Price Book</t>
-  </si>
-  <si>
-    <t>Buyer Price Book Home Page Close</t>
-  </si>
-  <si>
-    <t>TC016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verifying the customization of Price Book by removing the existing columns </t>
-  </si>
-  <si>
-    <t>Verify if it is able to Customize the Price book by removing the existing  column.</t>
-  </si>
-  <si>
-    <t>Verify if it is able to save the Price book by removing the provided column.</t>
-  </si>
-  <si>
-    <t>Verifying the Copy &amp; Paste feature of Price Book</t>
-  </si>
-  <si>
-    <t>Verify if it is able to Copy &amp; Paste the data from one Price Book to the New Price book</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Copy the existing Price book's data to a new Price book and save </t>
-  </si>
-  <si>
-    <t>Verify if it is able to save the Price book by copying  the existing Price Book's data to the new Price Book</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>There are no updates in price book</t>
-  </si>
-  <si>
-    <t>Price Book is empty</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="395">
+  <fills count="327">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -578,97 +581,7 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
+      <patternFill patternType="none">
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
@@ -699,271 +612,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
         <fgColor indexed="10"/>
       </patternFill>
     </fill>
@@ -973,7 +621,17 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="10"/>
       </patternFill>
     </fill>
@@ -983,297 +641,7 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
         <fgColor indexed="10"/>
       </patternFill>
     </fill>
@@ -1283,7 +651,7 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
         <fgColor indexed="10"/>
       </patternFill>
     </fill>
@@ -1293,297 +661,27 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="10"/>
       </patternFill>
     </fill>
@@ -1593,7 +691,32 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="10"/>
       </patternFill>
     </fill>
@@ -1603,207 +726,7 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
@@ -2114,6 +1037,26 @@
     </fill>
     <fill>
       <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
         <fgColor indexed="10"/>
       </patternFill>
     </fill>
@@ -2154,122 +1097,842 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
       </patternFill>
     </fill>
     <fill>
@@ -2552,7 +2215,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="240">
+  <cellXfs count="207">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
@@ -2627,36 +2290,37 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="7" fontId="4" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="8" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="8" fontId="5" numFmtId="49" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="17" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="18" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="23" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="25" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="27" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="28" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="29" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="31" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="32" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="34" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="9" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="11" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="14" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="16" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="18" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="20" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="22" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="35" fontId="5" numFmtId="49" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="24" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="26" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="28" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="30" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="31" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="36" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="38" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="35" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="37" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="38" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="40" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="44" fontId="0" numFmtId="0" xfId="0"/>
@@ -2800,41 +2464,7 @@
     <xf applyFill="true" borderId="0" fillId="320" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="322" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="true" borderId="0" fillId="324" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="326" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="328" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="330" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="332" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="334" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="336" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="338" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="340" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="342" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="344" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="346" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="348" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="350" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="352" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="354" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="356" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="358" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="360" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="362" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="364" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="366" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="368" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="370" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="372" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="374" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="376" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="378" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="380" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="382" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="384" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="386" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="388" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="390" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="true" borderId="0" fillId="392" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="394" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="326" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -3140,7 +2770,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3176,7 +2806,7 @@
         <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3189,7 +2819,7 @@
       <c r="C3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="219" t="s">
+      <c r="D3" s="177" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3203,7 +2833,7 @@
       <c r="C4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="221" t="s">
+      <c r="D4" s="179" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3217,7 +2847,7 @@
       <c r="C5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="225" t="s">
+      <c r="D5" s="183" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3231,7 +2861,7 @@
       <c r="C6" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="227" t="s">
+      <c r="D6" s="185" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3245,7 +2875,7 @@
       <c r="C7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="229" t="s">
+      <c r="D7" s="187" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3259,7 +2889,7 @@
       <c r="C8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="231" t="s">
+      <c r="D8" s="189" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3273,7 +2903,7 @@
       <c r="C9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="233" t="s">
+      <c r="D9" s="191" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3281,13 +2911,13 @@
       <c r="A10" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="32" t="s">
         <v>73</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="235" t="s">
+      <c r="D10" s="193" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3295,27 +2925,27 @@
       <c r="A11" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="32" t="s">
         <v>93</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="54" t="s">
-        <v>138</v>
+      <c r="B12" s="32" t="s">
+        <v>132</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="237" t="s">
+      <c r="D12" s="195" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3323,13 +2953,13 @@
       <c r="A13" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="54" t="s">
-        <v>139</v>
+      <c r="B13" s="32" t="s">
+        <v>133</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D13" t="s" s="239">
+      <c r="D13" s="197" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3337,13 +2967,13 @@
       <c r="A14" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B14" s="54" t="s">
-        <v>140</v>
+      <c r="B14" s="32" t="s">
+        <v>134</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="217" t="s">
+      <c r="D14" s="199" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3351,41 +2981,41 @@
       <c r="A15" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B15" s="54" t="s">
-        <v>141</v>
+      <c r="B15" s="32" t="s">
+        <v>135</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="148" t="s">
-        <v>134</v>
+      <c r="D15" s="201" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B16" s="54" t="s">
-        <v>142</v>
+      <c r="B16" s="32" t="s">
+        <v>136</v>
       </c>
       <c r="C16" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="151" t="s">
+      <c r="D16" s="204" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B17" s="54" t="s">
-        <v>143</v>
+        <v>138</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>137</v>
       </c>
       <c r="C17" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="153" t="s">
+      <c r="D17" t="s" s="206">
         <v>117</v>
       </c>
     </row>
@@ -3417,8 +3047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3508,7 +3138,7 @@
       <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="218" t="s">
+      <c r="D3" s="176" t="s">
         <v>117</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -3521,7 +3151,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -3540,7 +3170,7 @@
       <c r="C4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="220" t="s">
+      <c r="D4" s="178" t="s">
         <v>117</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -3576,7 +3206,7 @@
       <c r="C5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="222" t="s">
+      <c r="D5" s="180" t="s">
         <v>117</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -3620,7 +3250,7 @@
         <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>45</v>
@@ -3745,7 +3375,7 @@
       <c r="C2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="224" t="s">
+      <c r="D2" s="182" t="s">
         <v>117</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -3789,7 +3419,7 @@
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>47</v>
@@ -3927,7 +3557,7 @@
       <c r="C2" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="226" t="s">
+      <c r="D2" s="184" t="s">
         <v>117</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -4042,7 +3672,7 @@
       <c r="C2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="228" t="s">
+      <c r="D2" s="186" t="s">
         <v>117</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -4191,7 +3821,7 @@
       <c r="C2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="230" t="s">
+      <c r="D2" s="188" t="s">
         <v>117</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -4265,7 +3895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -4325,7 +3955,7 @@
       <c r="C2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="232" t="s">
+      <c r="D2" s="190" t="s">
         <v>117</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -4362,7 +3992,7 @@
         <v>64</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>151</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>47</v>
@@ -4387,7 +4017,7 @@
       <c r="C4" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="234" t="s">
+      <c r="D4" s="192" t="s">
         <v>117</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -4496,12 +4126,12 @@
         <v>92</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="236" t="s">
+      <c r="D8" s="194" t="s">
         <v>117</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -4554,12 +4184,12 @@
         <v>99</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="238" t="s">
+      <c r="D10" s="196" t="s">
         <v>117</v>
       </c>
       <c r="E10" s="11" t="s">
@@ -4622,25 +4252,25 @@
         <v>105</v>
       </c>
       <c r="K11" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="L11" s="11" t="s">
         <v>110</v>
       </c>
       <c r="M11" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="N11" s="11" t="s">
         <v>106</v>
       </c>
       <c r="O11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="P11" s="11" t="s">
         <v>107</v>
       </c>
       <c r="Q11" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
     </row>
     <row ht="45" r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -4648,12 +4278,12 @@
         <v>114</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="216" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="198" t="s">
         <v>117</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -4704,13 +4334,13 @@
         <v>115</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" s="147" t="s">
-        <v>134</v>
+      <c r="D14" s="200" t="s">
+        <v>117</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>118</v>
@@ -4762,7 +4392,7 @@
         <v>120</v>
       </c>
       <c r="G15" t="s">
-        <v>153</v>
+        <v>54</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>45</v>
@@ -4772,25 +4402,25 @@
         <v>105</v>
       </c>
       <c r="K15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="L15" s="11" t="s">
         <v>110</v>
       </c>
       <c r="M15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N15" s="11" t="s">
         <v>106</v>
       </c>
       <c r="O15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>107</v>
       </c>
       <c r="Q15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row ht="30" r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -4798,16 +4428,16 @@
         <v>116</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D16" s="149" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="202" t="s">
         <v>117</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>30</v>
@@ -4858,16 +4488,16 @@
         <v>116</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D18" s="150" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" s="203" t="s">
         <v>117</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F18" s="31" t="s">
         <v>42</v>
@@ -4901,10 +4531,10 @@
       <c r="D19" s="4"/>
       <c r="E19" s="11"/>
       <c r="F19" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G19" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>45</v>
@@ -4923,7 +4553,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>86</v>
@@ -4931,7 +4561,7 @@
       <c r="C20" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="152" t="s">
+      <c r="D20" s="205" t="s">
         <v>117</v>
       </c>
       <c r="E20" s="11" t="s">

</xml_diff>